<commit_message>
Added Assignment sheet Added pillar model
</commit_message>
<xml_diff>
--- a/CG - Final Assignment - Evaluation Form.xlsx
+++ b/CG - Final Assignment - Evaluation Form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\School\CG CPP\CG - Lecture 8 - 0 - Skeleton start\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F7C721-D248-4498-8310-1C4C85C551B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04AB588-2CFD-4385-9C61-CD257B76F71B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -347,9 +347,6 @@
     <t>A single designed object file for the pillars</t>
   </si>
   <si>
-    <t>Several textures implemented for many meshes (5+) and the ability to easily add textures to a model in the construction of a mesh or when calling .SetTexture</t>
-  </si>
-  <si>
     <t>2 unique animations defined for the rotation of showcase items (Rotating around a single axis, rotating around multiple axi)</t>
   </si>
   <si>
@@ -372,6 +369,9 @@
   </si>
   <si>
     <t>Several kinds of fragment shading defined using the Material class, several fragmentshaders used for imported models and primitive meshes, the floor reflects which can be seen when looking down</t>
+  </si>
+  <si>
+    <t>Several textures implemented for many meshes (5+) and the ability to easily add textures to a model in the construction of an obj or when calling .SetTexture</t>
   </si>
 </sst>
 </file>
@@ -1369,8 +1369,8 @@
   </sheetPr>
   <dimension ref="B2:M37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1624,7 +1624,7 @@
         <v>55</v>
       </c>
       <c r="M23" s="32" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="2:13" ht="57.6" x14ac:dyDescent="0.3">
@@ -1646,7 +1646,7 @@
         <v>56</v>
       </c>
       <c r="M24" s="32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="2:13" ht="86.4" x14ac:dyDescent="0.3">
@@ -1668,7 +1668,7 @@
         <v>77</v>
       </c>
       <c r="M25" s="32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="26" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
@@ -1690,7 +1690,7 @@
         <v>88</v>
       </c>
       <c r="M26" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="2:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
@@ -1710,7 +1710,7 @@
       </c>
       <c r="K27" s="50"/>
       <c r="M27" s="33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1759,7 +1759,7 @@
         <v>45</v>
       </c>
       <c r="M30" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="2:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1781,7 +1781,7 @@
         <v>42</v>
       </c>
       <c r="M31" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1846,7 +1846,7 @@
       </c>
       <c r="K35" s="41"/>
       <c r="M35" s="28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="2:13" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -1868,7 +1868,7 @@
         <v>69</v>
       </c>
       <c r="M36" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated some classes to prevent memory leaks
</commit_message>
<xml_diff>
--- a/CG - Final Assignment - Evaluation Form.xlsx
+++ b/CG - Final Assignment - Evaluation Form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\School\CG CPP\CG - Lecture 8 - 0 - Skeleton start\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D6F75D-73E2-4879-994C-1F9BA5BEC161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDED31C-F0F6-4489-B0D5-345CBE3F79AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="115">
   <si>
     <t>Knock-out criteria</t>
   </si>
@@ -372,6 +372,12 @@
   </si>
   <si>
     <t>Consistent naming based on concepts used, added comments to code to explain what the code does (In header files)</t>
+  </si>
+  <si>
+    <t>GPb</t>
+  </si>
+  <si>
+    <t>Note: Commented print from texture and model loaders to remove time spent on the I/O for console. In addition, glsl::readFile was rewritten to not leak memory so that a release build could be made. See OpenGL Final.exe for the compiled executable</t>
   </si>
 </sst>
 </file>
@@ -1369,8 +1375,8 @@
   </sheetPr>
   <dimension ref="B2:M37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D31" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1425,7 +1431,9 @@
       <c r="C6" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="38"/>
+      <c r="E6" s="38" t="s">
+        <v>113</v>
+      </c>
       <c r="F6" s="39"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.3">
@@ -1499,7 +1507,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:13" ht="100.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C17" s="1" t="s">
         <v>24</v>
       </c>
@@ -1510,7 +1518,9 @@
       <c r="F17" s="44"/>
       <c r="G17" s="45"/>
       <c r="H17" s="46"/>
-      <c r="M17" s="30"/>
+      <c r="M17" s="30" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="19" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
@@ -1561,7 +1571,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="2:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:13" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="4" t="s">
         <v>80</v>
       </c>

</xml_diff>